<commit_message>
fixing new OWID attributes and Micronesia
</commit_message>
<xml_diff>
--- a/data/GeoInformationWorld.xlsx
+++ b/data/GeoInformationWorld.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmbt/Documents/GitHub/Covid-19-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7309B27-FF74-4343-B2C2-C8118B028BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B3D316-D773-E149-B742-E46B9B0402AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{1C83CB90-EA5F-5941-9D13-79A5A21D1210}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="alpha2" localSheetId="0">Tabelle1!$A$1:$C$218</definedName>
+    <definedName name="alpha2" localSheetId="0">Tabelle1!$A$1:$C$219</definedName>
     <definedName name="tmp" localSheetId="0">Tabelle1!#REF!</definedName>
     <definedName name="tmp_1" localSheetId="0">Tabelle1!#REF!</definedName>
   </definedNames>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="666">
   <si>
     <t>GeoID</t>
   </si>
@@ -2045,6 +2045,15 @@
   </si>
   <si>
     <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>FSM</t>
   </si>
 </sst>
 </file>
@@ -2425,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7F271C-4077-C347-8A0A-5983B6691E37}">
-  <dimension ref="A1:F219"/>
+  <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="E201" sqref="E201"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4668,1500 +4677,1517 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="5" t="s">
+      <c r="A132" t="s">
+        <v>663</v>
+      </c>
+      <c r="B132" t="s">
+        <v>664</v>
+      </c>
+      <c r="C132" t="s">
+        <v>665</v>
+      </c>
+      <c r="D132" t="s">
+        <v>644</v>
+      </c>
+      <c r="E132">
+        <v>112640</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>371</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>372</v>
-      </c>
-      <c r="D132" t="s">
-        <v>641</v>
-      </c>
-      <c r="E132">
-        <v>4043258</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>374</v>
-      </c>
-      <c r="B133" t="s">
-        <v>373</v>
-      </c>
-      <c r="C133" t="s">
-        <v>375</v>
       </c>
       <c r="D133" t="s">
         <v>641</v>
       </c>
       <c r="E133">
-        <v>33085</v>
+        <v>4043258</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B134" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C134" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D134" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E134">
-        <v>3225166</v>
+        <v>33085</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B135" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C135" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D135" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E135">
-        <v>622182</v>
+        <v>3225166</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B136" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C136" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D136" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E136">
-        <v>4991</v>
+        <v>622182</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B137" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C137" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D137" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E137">
-        <v>36471766</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B138" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C138" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D138" t="s">
         <v>642</v>
       </c>
       <c r="E138">
-        <v>30366043</v>
+        <v>36471766</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B139" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C139" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D139" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E139">
-        <v>54045422</v>
+        <v>30366043</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>620</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>621</v>
+        <v>392</v>
+      </c>
+      <c r="B140" t="s">
+        <v>391</v>
       </c>
       <c r="C140" t="s">
-        <v>621</v>
+        <v>393</v>
       </c>
       <c r="D140" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E140">
-        <v>2494524</v>
+        <v>54045422</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>395</v>
-      </c>
-      <c r="B141" t="s">
-        <v>394</v>
+        <v>620</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>621</v>
       </c>
       <c r="C141" t="s">
-        <v>396</v>
+        <v>621</v>
       </c>
       <c r="D141" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E141">
-        <v>28608715</v>
+        <v>2494524</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B142" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C142" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D142" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E142">
-        <v>17282163</v>
+        <v>28608715</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B143" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C143" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D143" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E143">
-        <v>282757</v>
+        <v>17282163</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B144" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C144" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D144" t="s">
         <v>644</v>
       </c>
       <c r="E144">
-        <v>4783062</v>
+        <v>282757</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B145" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C145" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D145" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E145">
-        <v>6545503</v>
+        <v>4783062</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B146" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C146" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D146" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E146">
-        <v>23310719</v>
+        <v>6545503</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B147" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C147" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D147" t="s">
         <v>642</v>
       </c>
       <c r="E147">
-        <v>200963603</v>
+        <v>23310719</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B148" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C148" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D148" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E148">
-        <v>2077132</v>
+        <v>200963603</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B149" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C149" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D149" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E149">
-        <v>57213</v>
+        <v>2077132</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B150" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C150" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D150" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="E150">
-        <v>5328212</v>
+        <v>57213</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B151" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C151" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D151" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E151">
-        <v>4974992</v>
+        <v>5328212</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B152" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C152" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D152" t="s">
         <v>640</v>
       </c>
       <c r="E152">
-        <v>216565317</v>
+        <v>4974992</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>631</v>
+        <v>428</v>
       </c>
       <c r="B153" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C153" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D153" t="s">
         <v>640</v>
       </c>
       <c r="E153">
-        <v>4981422</v>
+        <v>216565317</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>433</v>
+        <v>631</v>
       </c>
       <c r="B154" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C154" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D154" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E154">
-        <v>4246440</v>
+        <v>4981422</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B155" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C155" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D155" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E155">
-        <v>8776119</v>
+        <v>4246440</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B156" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C156" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D156" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E156">
-        <v>7044639</v>
+        <v>8776119</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B157" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C157" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D157" t="s">
         <v>643</v>
       </c>
       <c r="E157">
-        <v>32510462</v>
+        <v>7044639</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B158" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C158" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D158" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="E158">
-        <v>108116622</v>
+        <v>32510462</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B159" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C159" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D159" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E159">
-        <v>37972812</v>
+        <v>108116622</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B160" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C160" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D160" t="s">
         <v>641</v>
       </c>
       <c r="E160">
-        <v>10276617</v>
+        <v>37972812</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B161" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C161" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D161" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E161">
-        <v>2933404</v>
+        <v>10276617</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B162" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C162" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D162" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="E162">
-        <v>2832071</v>
+        <v>2933404</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B163" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C163" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D163" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E163">
-        <v>19414458</v>
+        <v>2832071</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B164" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C164" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D164" t="s">
         <v>641</v>
       </c>
       <c r="E164">
-        <v>145872260</v>
+        <v>19414458</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B165" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C165" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D165" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E165">
-        <v>12626938</v>
+        <v>145872260</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B166" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C166" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D166" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E166">
-        <v>52834</v>
+        <v>12626938</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B167" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C167" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D167" t="s">
         <v>643</v>
       </c>
       <c r="E167">
-        <v>182795</v>
+        <v>52834</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B168" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C168" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D168" t="s">
         <v>643</v>
       </c>
       <c r="E168">
-        <v>110593</v>
-      </c>
-      <c r="F168" s="6"/>
+        <v>182795</v>
+      </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>656</v>
+        <v>475</v>
       </c>
       <c r="B169" t="s">
-        <v>654</v>
+        <v>474</v>
       </c>
       <c r="C169" t="s">
-        <v>655</v>
+        <v>476</v>
       </c>
       <c r="D169" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E169">
-        <v>180741</v>
+        <v>110593</v>
       </c>
       <c r="F169" s="6"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>478</v>
+        <v>656</v>
       </c>
       <c r="B170" t="s">
-        <v>477</v>
+        <v>654</v>
       </c>
       <c r="C170" t="s">
-        <v>479</v>
+        <v>655</v>
       </c>
       <c r="D170" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="E170">
-        <v>34453</v>
-      </c>
+        <v>180741</v>
+      </c>
+      <c r="F170" s="6"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B171" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C171" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D171" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E171">
-        <v>215048</v>
+        <v>34453</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B172" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C172" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D172" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E172">
-        <v>34268529</v>
+        <v>215048</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B173" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C173" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D173" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E173">
-        <v>16296362</v>
+        <v>34268529</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B174" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C174" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D174" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E174">
-        <v>6963764</v>
+        <v>16296362</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B175" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C175" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D175" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E175">
-        <v>97741</v>
+        <v>6963764</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B176" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C176" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D176" t="s">
         <v>642</v>
       </c>
       <c r="E176">
-        <v>7813207</v>
+        <v>97741</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B177" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C177" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D177" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E177">
-        <v>5804343</v>
+        <v>7813207</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B178" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C178" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D178" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E178">
-        <v>42389</v>
+        <v>5804343</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B179" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C179" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D179" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E179">
-        <v>5450421</v>
+        <v>42389</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B180" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C180" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D180" t="s">
         <v>641</v>
       </c>
       <c r="E180">
-        <v>2080908</v>
+        <v>5450421</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B181" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C181" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D181" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E181">
-        <v>669821</v>
+        <v>2080908</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B182" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C182" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D182" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E182">
-        <v>15442906</v>
+        <v>669821</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B183" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C183" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D183" t="s">
         <v>642</v>
       </c>
       <c r="E183">
-        <v>58558267</v>
+        <v>15442906</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>630</v>
+        <v>517</v>
       </c>
       <c r="B184" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C184" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D184" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E184">
-        <v>51225321</v>
+        <v>58558267</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>522</v>
+        <v>630</v>
       </c>
       <c r="B185" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C185" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D185" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E185">
-        <v>11062114</v>
+        <v>51225321</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B186" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C186" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D186" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E186">
-        <v>46937060</v>
+        <v>11062114</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B187" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C187" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D187" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E187">
-        <v>21323734</v>
+        <v>46937060</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B188" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C188" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D188" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E188">
-        <v>42813237</v>
+        <v>21323734</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B189" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C189" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D189" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E189">
-        <v>581363</v>
+        <v>42813237</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B190" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C190" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D190" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E190">
-        <v>10230185</v>
+        <v>581363</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B191" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C191" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D191" t="s">
         <v>641</v>
       </c>
       <c r="E191">
-        <v>8544527</v>
+        <v>10230185</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>540</v>
+      </c>
+      <c r="B192" t="s">
+        <v>539</v>
+      </c>
+      <c r="C192" t="s">
+        <v>541</v>
+      </c>
+      <c r="D192" t="s">
+        <v>641</v>
+      </c>
+      <c r="E192">
+        <v>8544527</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
         <v>543</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" t="s">
         <v>542</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C193" t="s">
         <v>544</v>
-      </c>
-      <c r="D192" t="s">
-        <v>640</v>
-      </c>
-      <c r="E192">
-        <v>17070132</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A193" s="5" t="s">
-        <v>629</v>
-      </c>
-      <c r="B193" t="s">
-        <v>545</v>
-      </c>
-      <c r="C193" t="s">
-        <v>546</v>
       </c>
       <c r="D193" t="s">
         <v>640</v>
       </c>
       <c r="E193">
-        <v>23773881</v>
+        <v>17070132</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>548</v>
+      <c r="A194" s="5" t="s">
+        <v>629</v>
       </c>
       <c r="B194" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C194" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D194" t="s">
         <v>640</v>
       </c>
       <c r="E194">
-        <v>9321023</v>
+        <v>23773881</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B195" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C195" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D195" t="s">
         <v>640</v>
       </c>
       <c r="E195">
-        <v>69625581</v>
+        <v>9321023</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B196" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C196" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D196" t="s">
         <v>640</v>
       </c>
       <c r="E196">
-        <v>1293120</v>
+        <v>69625581</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B197" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C197" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D197" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E197">
-        <v>8082359</v>
+        <v>1293120</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B198" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C198" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D198" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E198">
-        <v>1394969</v>
+        <v>8082359</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B199" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C199" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D199" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E199">
-        <v>11694721</v>
+        <v>1394969</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>563</v>
+      </c>
+      <c r="B200" t="s">
+        <v>562</v>
+      </c>
+      <c r="C200" t="s">
+        <v>564</v>
+      </c>
+      <c r="D200" t="s">
+        <v>642</v>
+      </c>
+      <c r="E200">
+        <v>11694721</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
         <v>566</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>565</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C201" t="s">
         <v>567</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D201" t="s">
         <v>641</v>
       </c>
-      <c r="E200">
+      <c r="E201">
         <v>82003882</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A201" s="6" t="s">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="6" t="s">
         <v>662</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>660</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C202" t="s">
         <v>661</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D202" t="s">
         <v>640</v>
       </c>
-      <c r="E201">
+      <c r="E202">
         <v>5942000</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
-        <v>569</v>
-      </c>
-      <c r="B202" t="s">
-        <v>568</v>
-      </c>
-      <c r="C202" t="s">
-        <v>570</v>
-      </c>
-      <c r="D202" t="s">
-        <v>643</v>
-      </c>
-      <c r="E202">
-        <v>38194</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B203" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C203" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D203" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E203">
-        <v>44269587</v>
+        <v>38194</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B204" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C204" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D204" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E204">
-        <v>43993643</v>
+        <v>44269587</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>575</v>
+      </c>
+      <c r="B205" t="s">
+        <v>574</v>
+      </c>
+      <c r="C205" t="s">
+        <v>576</v>
+      </c>
+      <c r="D205" t="s">
+        <v>641</v>
+      </c>
+      <c r="E205">
+        <v>43993643</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
         <v>578</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" t="s">
         <v>577</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C206" t="s">
         <v>579</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D206" t="s">
         <v>640</v>
       </c>
-      <c r="E205">
+      <c r="E206">
         <v>9770526</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A206" s="4" t="s">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B207" t="s">
         <v>622</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C207" t="s">
         <v>623</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D207" t="s">
         <v>641</v>
       </c>
-      <c r="E206">
+      <c r="E207">
         <v>66647112</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" s="5" t="s">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B208" t="s">
         <v>580</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C208" t="s">
         <v>581</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D208" t="s">
         <v>642</v>
       </c>
-      <c r="E207">
+      <c r="E208">
         <v>58005461</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
         <v>583</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B209" t="s">
         <v>582</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C209" t="s">
         <v>584</v>
-      </c>
-      <c r="D208" t="s">
-        <v>643</v>
-      </c>
-      <c r="E208">
-        <v>329064917</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209" s="5" t="s">
-        <v>627</v>
-      </c>
-      <c r="B209" t="s">
-        <v>585</v>
-      </c>
-      <c r="C209" t="s">
-        <v>586</v>
       </c>
       <c r="D209" t="s">
         <v>643</v>
       </c>
       <c r="E209">
-        <v>104579</v>
+        <v>329064917</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>588</v>
+      <c r="A210" s="5" t="s">
+        <v>627</v>
       </c>
       <c r="B210" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C210" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D210" t="s">
         <v>643</v>
       </c>
       <c r="E210">
-        <v>3461731</v>
+        <v>104579</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B211" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C211" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D211" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="E211">
-        <v>32981715</v>
+        <v>3461731</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>591</v>
+      </c>
+      <c r="B212" t="s">
+        <v>590</v>
+      </c>
+      <c r="C212" t="s">
+        <v>592</v>
+      </c>
+      <c r="D212" t="s">
+        <v>640</v>
+      </c>
+      <c r="E212">
+        <v>32981715</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
         <v>594</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B213" t="s">
         <v>593</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C213" t="s">
         <v>595</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D213" t="s">
         <v>644</v>
       </c>
-      <c r="E212">
+      <c r="E213">
         <v>299882</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" s="5" t="s">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" t="s">
         <v>596</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C214" t="s">
         <v>597</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D214" t="s">
         <v>643</v>
       </c>
-      <c r="E213">
+      <c r="E214">
         <v>28515829</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>599</v>
-      </c>
-      <c r="B214" t="s">
-        <v>598</v>
-      </c>
-      <c r="C214" t="s">
-        <v>600</v>
-      </c>
-      <c r="D214" t="s">
-        <v>640</v>
-      </c>
-      <c r="E214">
-        <v>96462108</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B215" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C215" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D215" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="E215">
-        <v>582458</v>
+        <v>96462108</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B216" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C216" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D216" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E216">
-        <v>29161922</v>
+        <v>582458</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B217" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C217" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D217" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E217">
-        <v>17861034</v>
+        <v>29161922</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B218" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C218" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D218" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E218">
-        <v>14645473</v>
+        <v>17861034</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
       <c r="B219" t="s">
-        <v>646</v>
+        <v>610</v>
       </c>
       <c r="C219" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="D219" t="s">
         <v>642</v>
       </c>
       <c r="E219">
+        <v>14645473</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>647</v>
+      </c>
+      <c r="B220" t="s">
+        <v>646</v>
+      </c>
+      <c r="C220" t="s">
+        <v>648</v>
+      </c>
+      <c r="D220" t="s">
+        <v>642</v>
+      </c>
+      <c r="E220">
         <v>16530000</v>
       </c>
     </row>

</xml_diff>